<commit_message>
improve the header detection accuraacry
</commit_message>
<xml_diff>
--- a/JF25034.xlsx
+++ b/JF25034.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\inv_pkl_contract_creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CA4B5BE-88C5-482E-9D39-51A1914F9564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD98DD3E-5175-4709-8870-7A80A8D402ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="116">
   <si>
     <t>客户公司名称：JASON FURNITURE VIET NAM COMPANY LIMITED</t>
   </si>
@@ -606,17 +606,38 @@
   <si>
     <t>01T25061804</t>
   </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>inv date</t>
+  </si>
+  <si>
+    <t>invoice no</t>
+  </si>
+  <si>
+    <t>invoice ref</t>
+  </si>
+  <si>
+    <t>invoice date</t>
+  </si>
+  <si>
+    <t>asdfafd</t>
+  </si>
+  <si>
+    <t>sdfasdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="0.00_ "/>
-    <numFmt numFmtId="169" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="171" formatCode="0.00;[Red]0.00"/>
-    <numFmt numFmtId="172" formatCode="0.000000_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
+    <numFmt numFmtId="165" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="167" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="168" formatCode="0.000000_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -867,7 +888,7 @@
     <xf numFmtId="40" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -894,7 +915,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -912,7 +933,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -927,10 +948,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -939,7 +960,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -954,11 +975,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -967,32 +988,50 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1005,24 +1044,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1514,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB49"/>
+  <dimension ref="A1:AC69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1533,27 +1554,27 @@
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125"/>
-    <col min="16" max="16" width="14.85546875" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125"/>
-    <col min="25" max="25" width="12.5703125"/>
-    <col min="27" max="27" width="12.5703125"/>
+    <col min="12" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125"/>
+    <col min="26" max="26" width="12.5703125"/>
+    <col min="28" max="28" width="12.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="36.950000000000003" customHeight="1">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="36.950000000000003" customHeight="1">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="67" t="s">
@@ -1562,12 +1583,12 @@
       <c r="H1" s="67"/>
       <c r="I1" s="67"/>
       <c r="J1" s="67"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="8"/>
-      <c r="Q1" s="43"/>
-      <c r="W1" s="43"/>
-    </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="O1" s="2"/>
+      <c r="P1" s="8"/>
+      <c r="R1" s="43"/>
+      <c r="X1" s="43"/>
+    </row>
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1585,14 +1606,15 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
-      <c r="N2" s="27"/>
+      <c r="N2" s="26"/>
       <c r="O2" s="27"/>
       <c r="P2" s="27"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="27"/>
-      <c r="W2" s="43"/>
-    </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="29.1" customHeight="1">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="27"/>
+      <c r="X2" s="43"/>
+    </row>
+    <row r="3" spans="1:29" s="1" customFormat="1" ht="29.1" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1612,20 +1634,21 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
-      <c r="N3" s="27"/>
+      <c r="N3" s="26"/>
       <c r="O3" s="27"/>
       <c r="P3" s="27"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="27"/>
-      <c r="W3" s="43"/>
-    </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="45.95" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="Q3" s="27"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="27"/>
+      <c r="X3" s="43"/>
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" ht="45.95" customHeight="1">
+      <c r="A4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="59"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="11"/>
       <c r="F4" s="5"/>
       <c r="G4" s="67"/>
@@ -1633,21 +1656,21 @@
       <c r="I4" s="67"/>
       <c r="J4" s="67"/>
       <c r="K4" s="26"/>
-      <c r="M4" s="27" t="s">
+      <c r="N4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="O4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="29">
+      <c r="P4" s="29">
         <f>B2</f>
         <v>45832</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="46"/>
-      <c r="W4" s="43"/>
-    </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="27.95" customHeight="1">
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
+      <c r="X4" s="43"/>
+    </row>
+    <row r="5" spans="1:29" s="1" customFormat="1" ht="27.95" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -1658,21 +1681,21 @@
       <c r="G5" s="11"/>
       <c r="H5" s="14"/>
       <c r="I5" s="13"/>
-      <c r="M5" s="30" t="s">
+      <c r="N5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="29">
-        <f>O4+1</f>
+      <c r="P5" s="29">
+        <f>P4+1</f>
         <v>45833</v>
       </c>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="47"/>
-      <c r="W5" s="43"/>
-    </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="27.95" customHeight="1">
+      <c r="R5" s="45"/>
+      <c r="S5" s="47"/>
+      <c r="X5" s="43"/>
+    </row>
+    <row r="6" spans="1:29" s="1" customFormat="1" ht="27.95" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1687,15 +1710,16 @@
       <c r="J6" s="13"/>
       <c r="K6" s="11"/>
       <c r="L6" s="14"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="8"/>
-      <c r="Q6" s="43"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="48"/>
-    </row>
-    <row r="7" spans="1:28" s="2" customFormat="1" ht="21" customHeight="1">
+      <c r="M6" s="14"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="8"/>
+      <c r="R6" s="43"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="48"/>
+    </row>
+    <row r="7" spans="1:29" s="2" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>13</v>
       </c>
@@ -1705,12 +1729,18 @@
       <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>109</v>
+      </c>
       <c r="F7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="H7" s="17" t="s">
         <v>16</v>
       </c>
@@ -1724,11 +1754,12 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="34"/>
-      <c r="T7" s="49"/>
-    </row>
-    <row r="8" spans="1:28" s="2" customFormat="1" ht="21" customHeight="1">
+      <c r="O7" s="17"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="34"/>
+      <c r="U7" s="49"/>
+    </row>
+    <row r="8" spans="1:29" s="2" customFormat="1" ht="21" customHeight="1">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1747,13 +1778,14 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="17"/>
+      <c r="P8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="34"/>
-      <c r="T8" s="49"/>
-    </row>
-    <row r="9" spans="1:28" s="3" customFormat="1" ht="45" customHeight="1">
+      <c r="Q8" s="34"/>
+      <c r="U8" s="49"/>
+    </row>
+    <row r="9" spans="1:29" s="3" customFormat="1" ht="45" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
@@ -1790,27 +1822,38 @@
       <c r="L9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="O9" s="37" t="s">
         <v>35</v>
-      </c>
-      <c r="O9" s="38" t="s">
-        <v>36</v>
       </c>
       <c r="P9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="Q9" s="50" t="s">
+      <c r="Q9" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="50" t="s">
+      <c r="S9" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="51"/>
-    </row>
-    <row r="10" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="T9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="U9" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A10" s="20" t="s">
         <v>39</v>
       </c>
@@ -1845,41 +1888,48 @@
         <v>10209.299999999999</v>
       </c>
       <c r="L10" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="M10" s="40">
         <v>1</v>
       </c>
-      <c r="M10" s="41">
-        <f>N10-45</f>
+      <c r="N10" s="41">
+        <f>O10-45</f>
         <v>768.5</v>
       </c>
-      <c r="N10" s="42">
+      <c r="O10" s="42">
         <v>813.5</v>
       </c>
-      <c r="O10" s="40">
+      <c r="P10" s="40">
         <v>1.25</v>
       </c>
-      <c r="P10" s="40">
-        <f t="shared" ref="P10:P48" si="0">O10*K10</f>
+      <c r="Q10" s="40">
+        <f t="shared" ref="Q10:Q48" si="0">P10*K10</f>
         <v>12761.625</v>
       </c>
-      <c r="Q10" s="42" t="s">
+      <c r="R10" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R10" s="40" t="s">
+      <c r="S10" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="S10" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="52"/>
+      <c r="T10" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="U10" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="V10" s="53" t="s">
+        <v>115</v>
+      </c>
       <c r="W10" s="52"/>
-      <c r="X10" s="54"/>
+      <c r="X10" s="52"/>
       <c r="Y10" s="54"/>
       <c r="Z10" s="54"/>
-      <c r="AB10" s="54"/>
-    </row>
-    <row r="11" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA10" s="54"/>
+      <c r="AC10" s="54"/>
+    </row>
+    <row r="11" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A11" s="20" t="s">
         <v>39</v>
       </c>
@@ -1914,41 +1964,44 @@
         <v>7398.2</v>
       </c>
       <c r="L11" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="M11" s="40">
         <v>1</v>
       </c>
-      <c r="M11" s="41">
-        <f>N11-45</f>
+      <c r="N11" s="41">
+        <f>O11-45</f>
         <v>568.5</v>
       </c>
-      <c r="N11" s="42">
+      <c r="O11" s="42">
         <v>613.5</v>
       </c>
-      <c r="O11" s="40">
+      <c r="P11" s="40">
         <v>1.25</v>
       </c>
-      <c r="P11" s="40">
+      <c r="Q11" s="40">
         <f t="shared" si="0"/>
         <v>9247.75</v>
       </c>
-      <c r="Q11" s="42" t="s">
+      <c r="R11" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R11" s="40" t="s">
+      <c r="S11" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="S11" s="40" t="s">
+      <c r="T11" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="T11" s="52"/>
-      <c r="U11" s="53"/>
-      <c r="V11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="53"/>
       <c r="W11" s="52"/>
-      <c r="X11" s="54"/>
+      <c r="X11" s="52"/>
       <c r="Y11" s="54"/>
       <c r="Z11" s="54"/>
-      <c r="AB11" s="54"/>
-    </row>
-    <row r="12" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA11" s="54"/>
+      <c r="AC11" s="54"/>
+    </row>
+    <row r="12" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A12" s="20" t="s">
         <v>52</v>
       </c>
@@ -1981,40 +2034,43 @@
         <v>10724.7</v>
       </c>
       <c r="L12" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="M12" s="40">
         <v>1</v>
       </c>
-      <c r="M12" s="41">
+      <c r="N12" s="41">
         <v>835.5</v>
       </c>
-      <c r="N12" s="42">
+      <c r="O12" s="42">
         <v>880.5</v>
       </c>
-      <c r="O12" s="40">
+      <c r="P12" s="40">
         <v>1.25</v>
       </c>
-      <c r="P12" s="40">
+      <c r="Q12" s="40">
         <f t="shared" si="0"/>
         <v>13405.875</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="R12" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R12" s="40" t="s">
+      <c r="S12" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="S12" s="40" t="s">
+      <c r="T12" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="T12" s="52"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="53"/>
       <c r="W12" s="52"/>
-      <c r="X12" s="54"/>
+      <c r="X12" s="52"/>
       <c r="Y12" s="54"/>
       <c r="Z12" s="54"/>
-      <c r="AB12" s="54"/>
-    </row>
-    <row r="13" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA12" s="54"/>
+      <c r="AC12" s="54"/>
+    </row>
+    <row r="13" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>52</v>
       </c>
@@ -2047,40 +2103,43 @@
         <v>10687.2</v>
       </c>
       <c r="L13" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="M13" s="40">
         <v>1</v>
       </c>
-      <c r="M13" s="41">
+      <c r="N13" s="41">
         <v>816</v>
       </c>
-      <c r="N13" s="42">
+      <c r="O13" s="42">
         <v>861</v>
       </c>
-      <c r="O13" s="40">
+      <c r="P13" s="40">
         <v>1.25</v>
       </c>
-      <c r="P13" s="40">
+      <c r="Q13" s="40">
         <f t="shared" si="0"/>
         <v>13359</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="R13" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R13" s="40" t="s">
+      <c r="S13" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="S13" s="40" t="s">
+      <c r="T13" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="T13" s="52"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="52"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="53"/>
       <c r="W13" s="52"/>
-      <c r="X13" s="54"/>
+      <c r="X13" s="52"/>
       <c r="Y13" s="54"/>
       <c r="Z13" s="54"/>
-      <c r="AB13" s="54"/>
-    </row>
-    <row r="14" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA13" s="54"/>
+      <c r="AC13" s="54"/>
+    </row>
+    <row r="14" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A14" s="20" t="s">
         <v>52</v>
       </c>
@@ -2112,41 +2171,44 @@
       <c r="K14" s="40">
         <v>7188.2</v>
       </c>
-      <c r="L14" s="61">
+      <c r="L14" s="40">
+        <v>7188.2</v>
+      </c>
+      <c r="M14" s="59">
         <v>1</v>
       </c>
-      <c r="M14" s="63">
+      <c r="N14" s="60">
         <v>562</v>
       </c>
-      <c r="N14" s="66">
+      <c r="O14" s="57">
         <v>607</v>
       </c>
-      <c r="O14" s="40">
+      <c r="P14" s="40">
         <v>1.25</v>
       </c>
-      <c r="P14" s="40">
+      <c r="Q14" s="40">
         <f t="shared" si="0"/>
         <v>8985.25</v>
       </c>
-      <c r="Q14" s="42" t="s">
+      <c r="R14" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R14" s="40" t="s">
+      <c r="S14" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="S14" s="40" t="s">
+      <c r="T14" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="T14" s="52"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="53"/>
       <c r="W14" s="52"/>
-      <c r="X14" s="54"/>
+      <c r="X14" s="52"/>
       <c r="Y14" s="54"/>
       <c r="Z14" s="54"/>
-      <c r="AB14" s="54"/>
-    </row>
-    <row r="15" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA14" s="54"/>
+      <c r="AC14" s="54"/>
+    </row>
+    <row r="15" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>52</v>
       </c>
@@ -2178,45 +2240,48 @@
       <c r="K15" s="40">
         <v>79.599999999999994</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="40">
+      <c r="L15" s="40">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="M15" s="58"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P15" s="40">
+      <c r="Q15" s="40">
         <f t="shared" si="0"/>
-        <v>89.947999999999993</v>
-      </c>
-      <c r="Q15" s="42" t="s">
+        <v>89.947999999999979</v>
+      </c>
+      <c r="R15" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40" t="s">
+      <c r="S15" s="40"/>
+      <c r="T15" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="T15" s="52">
+      <c r="U15" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="U15" s="55">
-        <f>T15-W15</f>
+      <c r="V15" s="55">
+        <f>U15-X15</f>
         <v>0</v>
       </c>
-      <c r="V15" s="56">
-        <f>O15-T15</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W15" s="52">
+      <c r="W15" s="56">
+        <f>P15-U15</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X15" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="X15" s="54"/>
       <c r="Y15" s="54"/>
       <c r="Z15" s="54"/>
-      <c r="AB15" s="54"/>
-    </row>
-    <row r="16" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA15" s="54"/>
+      <c r="AC15" s="54"/>
+    </row>
+    <row r="16" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A16" s="20" t="s">
         <v>52</v>
       </c>
@@ -2249,40 +2314,43 @@
         <v>11507.9</v>
       </c>
       <c r="L16" s="40">
+        <v>11507.9</v>
+      </c>
+      <c r="M16" s="40">
         <v>1</v>
       </c>
-      <c r="M16" s="41">
+      <c r="N16" s="41">
         <v>889</v>
       </c>
-      <c r="N16" s="42">
+      <c r="O16" s="42">
         <v>934</v>
       </c>
-      <c r="O16" s="40">
+      <c r="P16" s="40">
         <v>1.25</v>
       </c>
-      <c r="P16" s="40">
+      <c r="Q16" s="40">
         <f t="shared" si="0"/>
         <v>14384.875</v>
       </c>
-      <c r="Q16" s="42" t="s">
+      <c r="R16" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R16" s="40" t="s">
+      <c r="S16" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="S16" s="40" t="s">
+      <c r="T16" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="T16" s="52"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="52"/>
-      <c r="X16" s="54"/>
+      <c r="U16" s="52"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="52"/>
       <c r="Y16" s="54"/>
       <c r="Z16" s="54"/>
-      <c r="AB16" s="54"/>
-    </row>
-    <row r="17" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA16" s="54"/>
+      <c r="AC16" s="54"/>
+    </row>
+    <row r="17" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A17" s="20" t="s">
         <v>52</v>
       </c>
@@ -2315,40 +2383,43 @@
         <v>10652.9</v>
       </c>
       <c r="L17" s="40">
+        <v>10652.9</v>
+      </c>
+      <c r="M17" s="40">
         <v>1</v>
       </c>
-      <c r="M17" s="41">
+      <c r="N17" s="41">
         <v>827</v>
       </c>
-      <c r="N17" s="42">
+      <c r="O17" s="42">
         <v>872</v>
       </c>
-      <c r="O17" s="40">
+      <c r="P17" s="40">
         <v>1.25</v>
       </c>
-      <c r="P17" s="40">
+      <c r="Q17" s="40">
         <f t="shared" si="0"/>
         <v>13316.125</v>
       </c>
-      <c r="Q17" s="42" t="s">
+      <c r="R17" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="40" t="s">
+      <c r="S17" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="S17" s="40" t="s">
+      <c r="T17" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="T17" s="52"/>
-      <c r="U17" s="55"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="54"/>
+      <c r="U17" s="52"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="52"/>
       <c r="Y17" s="54"/>
       <c r="Z17" s="54"/>
-      <c r="AB17" s="54"/>
-    </row>
-    <row r="18" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA17" s="54"/>
+      <c r="AC17" s="54"/>
+    </row>
+    <row r="18" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A18" s="20" t="s">
         <v>52</v>
       </c>
@@ -2381,40 +2452,43 @@
         <v>10823.2</v>
       </c>
       <c r="L18" s="40">
+        <v>10823.2</v>
+      </c>
+      <c r="M18" s="40">
         <v>1</v>
       </c>
-      <c r="M18" s="41">
+      <c r="N18" s="41">
         <v>839.5</v>
       </c>
-      <c r="N18" s="42">
+      <c r="O18" s="42">
         <v>884.5</v>
       </c>
-      <c r="O18" s="40">
+      <c r="P18" s="40">
         <v>1.25</v>
       </c>
-      <c r="P18" s="40">
+      <c r="Q18" s="40">
         <f t="shared" si="0"/>
         <v>13529</v>
       </c>
-      <c r="Q18" s="42" t="s">
+      <c r="R18" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R18" s="40" t="s">
+      <c r="S18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="S18" s="40" t="s">
+      <c r="T18" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="T18" s="52"/>
-      <c r="U18" s="55"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="54"/>
+      <c r="U18" s="52"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="56"/>
+      <c r="X18" s="52"/>
       <c r="Y18" s="54"/>
       <c r="Z18" s="54"/>
-      <c r="AB18" s="54"/>
-    </row>
-    <row r="19" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA18" s="54"/>
+      <c r="AC18" s="54"/>
+    </row>
+    <row r="19" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A19" s="20" t="s">
         <v>52</v>
       </c>
@@ -2447,40 +2521,43 @@
         <v>10340.1</v>
       </c>
       <c r="L19" s="40">
+        <v>10340.1</v>
+      </c>
+      <c r="M19" s="40">
         <v>1</v>
       </c>
-      <c r="M19" s="41">
+      <c r="N19" s="41">
         <v>800</v>
       </c>
-      <c r="N19" s="42">
+      <c r="O19" s="42">
         <v>845</v>
       </c>
-      <c r="O19" s="40">
+      <c r="P19" s="40">
         <v>1.25</v>
       </c>
-      <c r="P19" s="40">
+      <c r="Q19" s="40">
         <f t="shared" si="0"/>
         <v>12925.125</v>
       </c>
-      <c r="Q19" s="42" t="s">
+      <c r="R19" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="40" t="s">
+      <c r="S19" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="S19" s="40" t="s">
+      <c r="T19" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="T19" s="52"/>
-      <c r="U19" s="55"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="52"/>
-      <c r="X19" s="54"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="55"/>
+      <c r="W19" s="56"/>
+      <c r="X19" s="52"/>
       <c r="Y19" s="54"/>
       <c r="Z19" s="54"/>
-      <c r="AB19" s="54"/>
-    </row>
-    <row r="20" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA19" s="54"/>
+      <c r="AC19" s="54"/>
+    </row>
+    <row r="20" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
@@ -2512,41 +2589,44 @@
       <c r="K20" s="40">
         <v>10124.5</v>
       </c>
-      <c r="L20" s="61">
+      <c r="L20" s="40">
+        <v>10124.5</v>
+      </c>
+      <c r="M20" s="59">
         <v>1</v>
       </c>
-      <c r="M20" s="63">
+      <c r="N20" s="60">
         <v>839.5</v>
       </c>
-      <c r="N20" s="66">
+      <c r="O20" s="57">
         <v>884.5</v>
       </c>
-      <c r="O20" s="40">
+      <c r="P20" s="40">
         <v>1.25</v>
       </c>
-      <c r="P20" s="40">
+      <c r="Q20" s="40">
         <f t="shared" si="0"/>
         <v>12655.625</v>
       </c>
-      <c r="Q20" s="42" t="s">
+      <c r="R20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R20" s="40" t="s">
+      <c r="S20" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="S20" s="40" t="s">
+      <c r="T20" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="T20" s="52"/>
-      <c r="U20" s="55"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="52"/>
-      <c r="X20" s="54"/>
+      <c r="U20" s="52"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="52"/>
       <c r="Y20" s="54"/>
       <c r="Z20" s="54"/>
-      <c r="AB20" s="54"/>
-    </row>
-    <row r="21" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA20" s="54"/>
+      <c r="AC20" s="54"/>
+    </row>
+    <row r="21" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A21" s="20" t="s">
         <v>52</v>
       </c>
@@ -2578,45 +2658,48 @@
       <c r="K21" s="40">
         <v>721.2</v>
       </c>
-      <c r="L21" s="62"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="40">
+      <c r="L21" s="40">
+        <v>721.2</v>
+      </c>
+      <c r="M21" s="58"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P21" s="40">
+      <c r="Q21" s="40">
         <f t="shared" si="0"/>
         <v>814.95600000000002</v>
       </c>
-      <c r="Q21" s="42" t="s">
+      <c r="R21" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40" t="s">
+      <c r="S21" s="40"/>
+      <c r="T21" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="T21" s="52">
+      <c r="U21" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="U21" s="55">
-        <f>T21-W21</f>
+      <c r="V21" s="55">
+        <f>U21-X21</f>
         <v>0</v>
       </c>
-      <c r="V21" s="56">
-        <f>O21-T21</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W21" s="52">
+      <c r="W21" s="56">
+        <f>P21-U21</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X21" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="X21" s="54"/>
       <c r="Y21" s="54"/>
       <c r="Z21" s="54"/>
-      <c r="AB21" s="54"/>
-    </row>
-    <row r="22" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA21" s="54"/>
+      <c r="AC21" s="54"/>
+    </row>
+    <row r="22" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A22" s="20" t="s">
         <v>52</v>
       </c>
@@ -2649,40 +2732,43 @@
         <v>10519.3</v>
       </c>
       <c r="L22" s="40">
+        <v>10519.3</v>
+      </c>
+      <c r="M22" s="40">
         <v>1</v>
       </c>
-      <c r="M22" s="41">
+      <c r="N22" s="41">
         <v>822.5</v>
       </c>
-      <c r="N22" s="42">
+      <c r="O22" s="42">
         <v>867.5</v>
       </c>
-      <c r="O22" s="40">
+      <c r="P22" s="40">
         <v>1.25</v>
       </c>
-      <c r="P22" s="40">
+      <c r="Q22" s="40">
         <f t="shared" si="0"/>
         <v>13149.125</v>
       </c>
-      <c r="Q22" s="42" t="s">
+      <c r="R22" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R22" s="40" t="s">
+      <c r="S22" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="S22" s="40" t="s">
+      <c r="T22" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="T22" s="52"/>
-      <c r="U22" s="55"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="54"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="56"/>
+      <c r="X22" s="52"/>
       <c r="Y22" s="54"/>
       <c r="Z22" s="54"/>
-      <c r="AB22" s="54"/>
-    </row>
-    <row r="23" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA22" s="54"/>
+      <c r="AC22" s="54"/>
+    </row>
+    <row r="23" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A23" s="20" t="s">
         <v>52</v>
       </c>
@@ -2715,40 +2801,43 @@
         <v>10625.2</v>
       </c>
       <c r="L23" s="40">
+        <v>10625.2</v>
+      </c>
+      <c r="M23" s="40">
         <v>1</v>
       </c>
-      <c r="M23" s="41">
+      <c r="N23" s="41">
         <v>823.5</v>
       </c>
-      <c r="N23" s="42">
+      <c r="O23" s="42">
         <v>868.5</v>
       </c>
-      <c r="O23" s="40">
+      <c r="P23" s="40">
         <v>1.25</v>
       </c>
-      <c r="P23" s="40">
+      <c r="Q23" s="40">
         <f t="shared" si="0"/>
         <v>13281.5</v>
       </c>
-      <c r="Q23" s="42" t="s">
+      <c r="R23" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R23" s="40" t="s">
+      <c r="S23" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="S23" s="40" t="s">
+      <c r="T23" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="T23" s="52"/>
-      <c r="U23" s="55"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="54"/>
+      <c r="U23" s="52"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="52"/>
       <c r="Y23" s="54"/>
       <c r="Z23" s="54"/>
-      <c r="AB23" s="54"/>
-    </row>
-    <row r="24" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA23" s="54"/>
+      <c r="AC23" s="54"/>
+    </row>
+    <row r="24" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>52</v>
       </c>
@@ -2781,40 +2870,43 @@
         <v>10195.5</v>
       </c>
       <c r="L24" s="40">
+        <v>10195.5</v>
+      </c>
+      <c r="M24" s="40">
         <v>1</v>
       </c>
-      <c r="M24" s="41">
+      <c r="N24" s="41">
         <v>798.5</v>
       </c>
-      <c r="N24" s="42">
+      <c r="O24" s="42">
         <v>843.5</v>
       </c>
-      <c r="O24" s="40">
+      <c r="P24" s="40">
         <v>1.25</v>
       </c>
-      <c r="P24" s="40">
+      <c r="Q24" s="40">
         <f t="shared" si="0"/>
         <v>12744.375</v>
       </c>
-      <c r="Q24" s="42" t="s">
+      <c r="R24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R24" s="40" t="s">
+      <c r="S24" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="S24" s="40" t="s">
+      <c r="T24" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="T24" s="52"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="54"/>
+      <c r="U24" s="52"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="56"/>
+      <c r="X24" s="52"/>
       <c r="Y24" s="54"/>
       <c r="Z24" s="54"/>
-      <c r="AB24" s="54"/>
-    </row>
-    <row r="25" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA24" s="54"/>
+      <c r="AC24" s="54"/>
+    </row>
+    <row r="25" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A25" s="20" t="s">
         <v>52</v>
       </c>
@@ -2846,41 +2938,44 @@
       <c r="K25" s="40">
         <v>8854.9</v>
       </c>
-      <c r="L25" s="61">
+      <c r="L25" s="40">
+        <v>8854.9</v>
+      </c>
+      <c r="M25" s="59">
         <v>1</v>
       </c>
-      <c r="M25" s="63">
+      <c r="N25" s="60">
         <v>733.5</v>
       </c>
-      <c r="N25" s="66">
+      <c r="O25" s="57">
         <v>778.5</v>
       </c>
-      <c r="O25" s="40">
+      <c r="P25" s="40">
         <v>1.25</v>
       </c>
-      <c r="P25" s="40">
+      <c r="Q25" s="40">
         <f t="shared" si="0"/>
         <v>11068.625</v>
       </c>
-      <c r="Q25" s="42" t="s">
+      <c r="R25" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R25" s="40" t="s">
+      <c r="S25" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="S25" s="40" t="s">
+      <c r="T25" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="T25" s="52"/>
-      <c r="U25" s="55"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="52"/>
-      <c r="X25" s="54"/>
+      <c r="U25" s="52"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="56"/>
+      <c r="X25" s="52"/>
       <c r="Y25" s="54"/>
       <c r="Z25" s="54"/>
-      <c r="AB25" s="54"/>
-    </row>
-    <row r="26" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA25" s="54"/>
+      <c r="AC25" s="54"/>
+    </row>
+    <row r="26" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A26" s="20" t="s">
         <v>52</v>
       </c>
@@ -2912,45 +3007,48 @@
       <c r="K26" s="40">
         <v>566.9</v>
       </c>
-      <c r="L26" s="62"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="40">
+      <c r="L26" s="40">
+        <v>566.9</v>
+      </c>
+      <c r="M26" s="58"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P26" s="40">
+      <c r="Q26" s="40">
         <f t="shared" si="0"/>
-        <v>640.59699999999998</v>
-      </c>
-      <c r="Q26" s="42" t="s">
+        <v>640.59699999999987</v>
+      </c>
+      <c r="R26" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40" t="s">
+      <c r="S26" s="40"/>
+      <c r="T26" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="T26" s="52">
+      <c r="U26" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="U26" s="55">
-        <f t="shared" ref="U26:U29" si="1">T26-W26</f>
+      <c r="V26" s="55">
+        <f t="shared" ref="V26:V29" si="1">U26-X26</f>
         <v>0</v>
       </c>
-      <c r="V26" s="56">
-        <f t="shared" ref="V26:V29" si="2">O26-T26</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W26" s="52">
+      <c r="W26" s="56">
+        <f t="shared" ref="W26:W29" si="2">P26-U26</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X26" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="X26" s="54"/>
       <c r="Y26" s="54"/>
       <c r="Z26" s="54"/>
-      <c r="AB26" s="54"/>
-    </row>
-    <row r="27" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA26" s="54"/>
+      <c r="AC26" s="54"/>
+    </row>
+    <row r="27" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A27" s="20" t="s">
         <v>52</v>
       </c>
@@ -2982,41 +3080,44 @@
       <c r="K27" s="40">
         <v>8935.7999999999993</v>
       </c>
-      <c r="L27" s="61">
+      <c r="L27" s="40">
+        <v>8935.7999999999993</v>
+      </c>
+      <c r="M27" s="59">
         <v>1</v>
       </c>
-      <c r="M27" s="63">
+      <c r="N27" s="60">
         <v>763</v>
       </c>
-      <c r="N27" s="66">
+      <c r="O27" s="57">
         <v>808</v>
       </c>
-      <c r="O27" s="40">
+      <c r="P27" s="40">
         <v>1.25</v>
       </c>
-      <c r="P27" s="40">
+      <c r="Q27" s="40">
         <f t="shared" si="0"/>
         <v>11169.75</v>
       </c>
-      <c r="Q27" s="42" t="s">
+      <c r="R27" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R27" s="40" t="s">
+      <c r="S27" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="S27" s="40" t="s">
+      <c r="T27" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="T27" s="52"/>
-      <c r="U27" s="55"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="54"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="56"/>
+      <c r="X27" s="52"/>
       <c r="Y27" s="54"/>
       <c r="Z27" s="54"/>
-      <c r="AB27" s="54"/>
-    </row>
-    <row r="28" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA27" s="54"/>
+      <c r="AC27" s="54"/>
+    </row>
+    <row r="28" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A28" s="20" t="s">
         <v>52</v>
       </c>
@@ -3048,45 +3149,48 @@
       <c r="K28" s="40">
         <v>316.89999999999998</v>
       </c>
-      <c r="L28" s="61"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="40">
+      <c r="L28" s="40">
+        <v>316.89999999999998</v>
+      </c>
+      <c r="M28" s="59"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="P28" s="40">
+      <c r="Q28" s="40">
         <f t="shared" si="0"/>
-        <v>358.09699999999998</v>
-      </c>
-      <c r="Q28" s="42" t="s">
+        <v>358.09699999999992</v>
+      </c>
+      <c r="R28" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40" t="s">
+      <c r="S28" s="40"/>
+      <c r="T28" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="T28" s="52">
+      <c r="U28" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="U28" s="55">
+      <c r="V28" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V28" s="56">
+      <c r="W28" s="56">
         <f t="shared" si="2"/>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W28" s="52">
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X28" s="52">
         <f>1.25*0.9</f>
         <v>1.125</v>
       </c>
-      <c r="X28" s="54"/>
       <c r="Y28" s="54"/>
       <c r="Z28" s="54"/>
-      <c r="AB28" s="54"/>
-    </row>
-    <row r="29" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA28" s="54"/>
+      <c r="AC28" s="54"/>
+    </row>
+    <row r="29" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
@@ -3118,45 +3222,48 @@
       <c r="K29" s="40">
         <v>659.6</v>
       </c>
-      <c r="L29" s="62"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="40">
+      <c r="L29" s="40">
+        <v>659.6</v>
+      </c>
+      <c r="M29" s="58"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="40">
         <v>1.06</v>
       </c>
-      <c r="P29" s="40">
+      <c r="Q29" s="40">
         <f t="shared" si="0"/>
         <v>699.17600000000004</v>
       </c>
-      <c r="Q29" s="42" t="s">
+      <c r="R29" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40" t="s">
+      <c r="S29" s="40"/>
+      <c r="T29" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="T29" s="52">
+      <c r="U29" s="52">
         <f>1.25*0.85</f>
         <v>1.0625</v>
       </c>
-      <c r="U29" s="55">
+      <c r="V29" s="55">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V29" s="56">
+      <c r="W29" s="56">
         <f t="shared" si="2"/>
-        <v>-2.4999999999999502E-3</v>
-      </c>
-      <c r="W29" s="52">
+        <v>-2.4999999999999467E-3</v>
+      </c>
+      <c r="X29" s="52">
         <f>1.25*0.85</f>
         <v>1.0625</v>
       </c>
-      <c r="X29" s="54"/>
       <c r="Y29" s="54"/>
       <c r="Z29" s="54"/>
-      <c r="AB29" s="54"/>
-    </row>
-    <row r="30" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA29" s="54"/>
+      <c r="AC29" s="54"/>
+    </row>
+    <row r="30" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A30" s="20" t="s">
         <v>52</v>
       </c>
@@ -3189,41 +3296,44 @@
         <v>1718.4</v>
       </c>
       <c r="L30" s="40">
+        <v>1718.4</v>
+      </c>
+      <c r="M30" s="40">
         <v>1</v>
       </c>
-      <c r="M30" s="41">
-        <f>N30+45</f>
+      <c r="N30" s="41">
+        <f>O30+45</f>
         <v>197</v>
       </c>
-      <c r="N30" s="42">
+      <c r="O30" s="42">
         <v>152</v>
       </c>
-      <c r="O30" s="40">
+      <c r="P30" s="40">
         <v>1.25</v>
       </c>
-      <c r="P30" s="40">
+      <c r="Q30" s="40">
         <f t="shared" si="0"/>
         <v>2148</v>
       </c>
-      <c r="Q30" s="42" t="s">
+      <c r="R30" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R30" s="40" t="s">
+      <c r="S30" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="S30" s="40" t="s">
+      <c r="T30" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="T30" s="52"/>
-      <c r="U30" s="55"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="52"/>
-      <c r="X30" s="54"/>
+      <c r="U30" s="52"/>
+      <c r="V30" s="55"/>
+      <c r="W30" s="56"/>
+      <c r="X30" s="52"/>
       <c r="Y30" s="54"/>
       <c r="Z30" s="54"/>
-      <c r="AB30" s="54"/>
-    </row>
-    <row r="31" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA30" s="54"/>
+      <c r="AC30" s="54"/>
+    </row>
+    <row r="31" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A31" s="20" t="s">
         <v>83</v>
       </c>
@@ -3256,40 +3366,43 @@
         <v>5010</v>
       </c>
       <c r="L31" s="40">
+        <v>5010</v>
+      </c>
+      <c r="M31" s="40">
         <v>1</v>
       </c>
-      <c r="M31" s="41">
+      <c r="N31" s="41">
         <v>443.5</v>
       </c>
-      <c r="N31" s="42">
+      <c r="O31" s="42">
         <v>488.5</v>
       </c>
-      <c r="O31" s="40">
+      <c r="P31" s="40">
         <v>1.05</v>
       </c>
-      <c r="P31" s="40">
+      <c r="Q31" s="40">
         <f t="shared" si="0"/>
         <v>5260.5</v>
       </c>
-      <c r="Q31" s="42" t="s">
+      <c r="R31" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R31" s="40" t="s">
+      <c r="S31" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="S31" s="40" t="s">
+      <c r="T31" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="T31" s="52"/>
-      <c r="U31" s="55"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="54"/>
+      <c r="U31" s="52"/>
+      <c r="V31" s="55"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="52"/>
       <c r="Y31" s="54"/>
       <c r="Z31" s="54"/>
-      <c r="AB31" s="54"/>
-    </row>
-    <row r="32" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA31" s="54"/>
+      <c r="AC31" s="54"/>
+    </row>
+    <row r="32" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A32" s="20" t="s">
         <v>83</v>
       </c>
@@ -3322,40 +3435,43 @@
         <v>5018.8</v>
       </c>
       <c r="L32" s="40">
+        <v>5018.8</v>
+      </c>
+      <c r="M32" s="40">
         <v>1</v>
       </c>
-      <c r="M32" s="41">
+      <c r="N32" s="41">
         <v>445.5</v>
       </c>
-      <c r="N32" s="42">
+      <c r="O32" s="42">
         <v>490.5</v>
       </c>
-      <c r="O32" s="40">
+      <c r="P32" s="40">
         <v>1.05</v>
       </c>
-      <c r="P32" s="40">
+      <c r="Q32" s="40">
         <f t="shared" si="0"/>
-        <v>5269.74</v>
-      </c>
-      <c r="Q32" s="42" t="s">
+        <v>5269.7400000000007</v>
+      </c>
+      <c r="R32" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R32" s="40" t="s">
+      <c r="S32" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="S32" s="40" t="s">
+      <c r="T32" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="T32" s="52"/>
-      <c r="U32" s="55"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="54"/>
+      <c r="U32" s="52"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="56"/>
+      <c r="X32" s="52"/>
       <c r="Y32" s="54"/>
       <c r="Z32" s="54"/>
-      <c r="AB32" s="54"/>
-    </row>
-    <row r="33" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA32" s="54"/>
+      <c r="AC32" s="54"/>
+    </row>
+    <row r="33" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A33" s="20" t="s">
         <v>91</v>
       </c>
@@ -3387,41 +3503,44 @@
       <c r="K33" s="40">
         <v>8994.2999999999993</v>
       </c>
-      <c r="L33" s="61">
+      <c r="L33" s="40">
+        <v>8994.2999999999993</v>
+      </c>
+      <c r="M33" s="59">
         <v>1</v>
       </c>
-      <c r="M33" s="63">
+      <c r="N33" s="60">
         <v>986</v>
       </c>
-      <c r="N33" s="66">
+      <c r="O33" s="57">
         <v>1031</v>
       </c>
-      <c r="O33" s="40">
+      <c r="P33" s="40">
         <v>1.05</v>
       </c>
-      <c r="P33" s="40">
+      <c r="Q33" s="40">
         <f t="shared" si="0"/>
         <v>9444.0149999999994</v>
       </c>
-      <c r="Q33" s="42" t="s">
+      <c r="R33" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R33" s="40" t="s">
+      <c r="S33" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="S33" s="40" t="s">
+      <c r="T33" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="T33" s="52"/>
-      <c r="U33" s="55"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="54"/>
+      <c r="U33" s="52"/>
+      <c r="V33" s="55"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="52"/>
       <c r="Y33" s="54"/>
       <c r="Z33" s="54"/>
-      <c r="AB33" s="54"/>
-    </row>
-    <row r="34" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA33" s="54"/>
+      <c r="AC33" s="54"/>
+    </row>
+    <row r="34" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A34" s="20" t="s">
         <v>91</v>
       </c>
@@ -3453,45 +3572,48 @@
       <c r="K34" s="40">
         <v>394.6</v>
       </c>
-      <c r="L34" s="61"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="40">
+      <c r="L34" s="40">
+        <v>394.6</v>
+      </c>
+      <c r="M34" s="59"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="59"/>
+      <c r="P34" s="40">
         <v>0.95</v>
       </c>
-      <c r="P34" s="40">
+      <c r="Q34" s="40">
         <f t="shared" si="0"/>
         <v>374.87</v>
       </c>
-      <c r="Q34" s="42" t="s">
+      <c r="R34" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40" t="s">
+      <c r="S34" s="40"/>
+      <c r="T34" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="T34" s="52">
+      <c r="U34" s="52">
         <f>1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="U34" s="55">
-        <f>T34-W34</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V34" s="55">
+        <f>U34-X34</f>
         <v>0</v>
       </c>
-      <c r="V34" s="56">
-        <f>O34-T34</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W34" s="52">
+      <c r="W34" s="56">
+        <f>P34-U34</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X34" s="52">
         <f>1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="X34" s="54"/>
+        <v>0.94500000000000006</v>
+      </c>
       <c r="Y34" s="54"/>
       <c r="Z34" s="54"/>
-      <c r="AB34" s="54"/>
-    </row>
-    <row r="35" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA34" s="54"/>
+      <c r="AC34" s="54"/>
+    </row>
+    <row r="35" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A35" s="20" t="s">
         <v>91</v>
       </c>
@@ -3523,45 +3645,48 @@
       <c r="K35" s="40">
         <v>1695.3</v>
       </c>
-      <c r="L35" s="62"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="40">
+      <c r="L35" s="40">
+        <v>1695.3</v>
+      </c>
+      <c r="M35" s="58"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="40">
         <v>0.89</v>
       </c>
-      <c r="P35" s="40">
+      <c r="Q35" s="40">
         <f t="shared" si="0"/>
         <v>1508.817</v>
       </c>
-      <c r="Q35" s="42" t="s">
+      <c r="R35" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R35" s="40"/>
-      <c r="S35" s="40" t="s">
+      <c r="S35" s="40"/>
+      <c r="T35" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="T35" s="52">
+      <c r="U35" s="52">
         <f>1.05*0.85</f>
         <v>0.89249999999999996</v>
       </c>
-      <c r="U35" s="55">
-        <f>T35-W35</f>
+      <c r="V35" s="55">
+        <f>U35-X35</f>
         <v>0</v>
       </c>
-      <c r="V35" s="56">
-        <f>O35-T35</f>
-        <v>-2.4999999999999502E-3</v>
-      </c>
-      <c r="W35" s="52">
+      <c r="W35" s="56">
+        <f>P35-U35</f>
+        <v>-2.4999999999999467E-3</v>
+      </c>
+      <c r="X35" s="52">
         <f>1.05*0.85</f>
         <v>0.89249999999999996</v>
       </c>
-      <c r="X35" s="54"/>
       <c r="Y35" s="54"/>
       <c r="Z35" s="54"/>
-      <c r="AB35" s="54"/>
-    </row>
-    <row r="36" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA35" s="54"/>
+      <c r="AC35" s="54"/>
+    </row>
+    <row r="36" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A36" s="20" t="s">
         <v>95</v>
       </c>
@@ -3594,40 +3719,43 @@
         <v>10947.2</v>
       </c>
       <c r="L36" s="40">
+        <v>10947.2</v>
+      </c>
+      <c r="M36" s="40">
         <v>1</v>
       </c>
-      <c r="M36" s="41">
+      <c r="N36" s="41">
         <v>963</v>
       </c>
-      <c r="N36" s="42">
+      <c r="O36" s="42">
         <v>1008</v>
       </c>
-      <c r="O36" s="40">
+      <c r="P36" s="40">
         <v>1.05</v>
       </c>
-      <c r="P36" s="40">
+      <c r="Q36" s="40">
         <f t="shared" si="0"/>
-        <v>11494.56</v>
-      </c>
-      <c r="Q36" s="42" t="s">
+        <v>11494.560000000001</v>
+      </c>
+      <c r="R36" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R36" s="40" t="s">
+      <c r="S36" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="S36" s="40" t="s">
+      <c r="T36" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="T36" s="52"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="56"/>
-      <c r="W36" s="52"/>
-      <c r="X36" s="54"/>
+      <c r="U36" s="52"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="56"/>
+      <c r="X36" s="52"/>
       <c r="Y36" s="54"/>
       <c r="Z36" s="54"/>
-      <c r="AB36" s="54"/>
-    </row>
-    <row r="37" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA36" s="54"/>
+      <c r="AC36" s="54"/>
+    </row>
+    <row r="37" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A37" s="20" t="s">
         <v>95</v>
       </c>
@@ -3660,40 +3788,43 @@
         <v>10962.5</v>
       </c>
       <c r="L37" s="40">
+        <v>10962.5</v>
+      </c>
+      <c r="M37" s="40">
         <v>1</v>
       </c>
-      <c r="M37" s="41">
+      <c r="N37" s="41">
         <v>970.5</v>
       </c>
-      <c r="N37" s="42">
+      <c r="O37" s="42">
         <v>1015.5</v>
       </c>
-      <c r="O37" s="40">
+      <c r="P37" s="40">
         <v>1.05</v>
       </c>
-      <c r="P37" s="40">
+      <c r="Q37" s="40">
         <f t="shared" si="0"/>
         <v>11510.625</v>
       </c>
-      <c r="Q37" s="42" t="s">
+      <c r="R37" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R37" s="40" t="s">
+      <c r="S37" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="S37" s="40" t="s">
+      <c r="T37" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="T37" s="52"/>
-      <c r="U37" s="55"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="52"/>
-      <c r="X37" s="54"/>
+      <c r="U37" s="52"/>
+      <c r="V37" s="55"/>
+      <c r="W37" s="56"/>
+      <c r="X37" s="52"/>
       <c r="Y37" s="54"/>
       <c r="Z37" s="54"/>
-      <c r="AB37" s="54"/>
-    </row>
-    <row r="38" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA37" s="54"/>
+      <c r="AC37" s="54"/>
+    </row>
+    <row r="38" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A38" s="20" t="s">
         <v>95</v>
       </c>
@@ -3726,40 +3857,43 @@
         <v>10895.3</v>
       </c>
       <c r="L38" s="40">
+        <v>10895.3</v>
+      </c>
+      <c r="M38" s="40">
         <v>1</v>
       </c>
-      <c r="M38" s="41">
+      <c r="N38" s="41">
         <v>955</v>
       </c>
-      <c r="N38" s="42">
+      <c r="O38" s="42">
         <v>1000</v>
       </c>
-      <c r="O38" s="40">
+      <c r="P38" s="40">
         <v>1.05</v>
       </c>
-      <c r="P38" s="40">
+      <c r="Q38" s="40">
         <f t="shared" si="0"/>
         <v>11440.065000000001</v>
       </c>
-      <c r="Q38" s="42" t="s">
+      <c r="R38" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R38" s="40" t="s">
+      <c r="S38" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="S38" s="40" t="s">
+      <c r="T38" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="T38" s="52"/>
-      <c r="U38" s="55"/>
-      <c r="V38" s="56"/>
-      <c r="W38" s="52"/>
-      <c r="X38" s="54"/>
+      <c r="U38" s="52"/>
+      <c r="V38" s="55"/>
+      <c r="W38" s="56"/>
+      <c r="X38" s="52"/>
       <c r="Y38" s="54"/>
       <c r="Z38" s="54"/>
-      <c r="AB38" s="54"/>
-    </row>
-    <row r="39" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA38" s="54"/>
+      <c r="AC38" s="54"/>
+    </row>
+    <row r="39" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A39" s="20" t="s">
         <v>95</v>
       </c>
@@ -3791,41 +3925,44 @@
       <c r="K39" s="40">
         <v>10077.299999999999</v>
       </c>
-      <c r="L39" s="61">
+      <c r="L39" s="40">
+        <v>10077.299999999999</v>
+      </c>
+      <c r="M39" s="59">
         <v>1</v>
       </c>
-      <c r="M39" s="63">
+      <c r="N39" s="60">
         <v>965.5</v>
       </c>
-      <c r="N39" s="66">
+      <c r="O39" s="57">
         <v>1010.5</v>
       </c>
-      <c r="O39" s="40">
+      <c r="P39" s="40">
         <v>1.05</v>
       </c>
-      <c r="P39" s="40">
+      <c r="Q39" s="40">
         <f t="shared" si="0"/>
-        <v>10581.165000000001</v>
-      </c>
-      <c r="Q39" s="42" t="s">
+        <v>10581.164999999999</v>
+      </c>
+      <c r="R39" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R39" s="40" t="s">
+      <c r="S39" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="S39" s="40" t="s">
+      <c r="T39" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="T39" s="52"/>
-      <c r="U39" s="55"/>
-      <c r="V39" s="56"/>
-      <c r="W39" s="52"/>
-      <c r="X39" s="54"/>
+      <c r="U39" s="52"/>
+      <c r="V39" s="55"/>
+      <c r="W39" s="56"/>
+      <c r="X39" s="52"/>
       <c r="Y39" s="54"/>
       <c r="Z39" s="54"/>
-      <c r="AB39" s="54"/>
-    </row>
-    <row r="40" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA39" s="54"/>
+      <c r="AC39" s="54"/>
+    </row>
+    <row r="40" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A40" s="20" t="s">
         <v>95</v>
       </c>
@@ -3857,45 +3994,48 @@
       <c r="K40" s="40">
         <v>905.2</v>
       </c>
-      <c r="L40" s="62"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="40">
+      <c r="L40" s="40">
+        <v>905.2</v>
+      </c>
+      <c r="M40" s="58"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="40">
         <v>0.95</v>
       </c>
-      <c r="P40" s="40">
+      <c r="Q40" s="40">
         <f t="shared" si="0"/>
         <v>859.94</v>
       </c>
-      <c r="Q40" s="42" t="s">
+      <c r="R40" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R40" s="40"/>
-      <c r="S40" s="40" t="s">
+      <c r="S40" s="40"/>
+      <c r="T40" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="T40" s="52">
+      <c r="U40" s="52">
         <f>1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="U40" s="55">
-        <f t="shared" ref="U40:U44" si="3">T40-W40</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V40" s="55">
+        <f t="shared" ref="V40:V44" si="3">U40-X40</f>
         <v>0</v>
       </c>
-      <c r="V40" s="56">
-        <f t="shared" ref="V40:V44" si="4">O40-T40</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W40" s="52">
+      <c r="W40" s="56">
+        <f t="shared" ref="W40:W44" si="4">P40-U40</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X40" s="52">
         <f>1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="X40" s="54"/>
+        <v>0.94500000000000006</v>
+      </c>
       <c r="Y40" s="54"/>
       <c r="Z40" s="54"/>
-      <c r="AB40" s="54"/>
-    </row>
-    <row r="41" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA40" s="54"/>
+      <c r="AC40" s="54"/>
+    </row>
+    <row r="41" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A41" s="20" t="s">
         <v>95</v>
       </c>
@@ -3927,41 +4067,44 @@
       <c r="K41" s="40">
         <v>8517.7000000000007</v>
       </c>
-      <c r="L41" s="61">
+      <c r="L41" s="40">
+        <v>8517.7000000000007</v>
+      </c>
+      <c r="M41" s="59">
         <v>1</v>
       </c>
-      <c r="M41" s="63">
+      <c r="N41" s="60">
         <v>839</v>
       </c>
-      <c r="N41" s="66">
+      <c r="O41" s="57">
         <v>884</v>
       </c>
-      <c r="O41" s="40">
+      <c r="P41" s="40">
         <v>1.05</v>
       </c>
-      <c r="P41" s="40">
+      <c r="Q41" s="40">
         <f t="shared" si="0"/>
-        <v>8943.5849999999991</v>
-      </c>
-      <c r="Q41" s="42" t="s">
+        <v>8943.5850000000009</v>
+      </c>
+      <c r="R41" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R41" s="40" t="s">
+      <c r="S41" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="S41" s="40" t="s">
+      <c r="T41" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="T41" s="52"/>
-      <c r="U41" s="55"/>
-      <c r="V41" s="56"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="54"/>
+      <c r="U41" s="52"/>
+      <c r="V41" s="55"/>
+      <c r="W41" s="56"/>
+      <c r="X41" s="52"/>
       <c r="Y41" s="54"/>
       <c r="Z41" s="54"/>
-      <c r="AB41" s="54"/>
-    </row>
-    <row r="42" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA41" s="54"/>
+      <c r="AC41" s="54"/>
+    </row>
+    <row r="42" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A42" s="20" t="s">
         <v>95</v>
       </c>
@@ -3993,45 +4136,48 @@
       <c r="K42" s="40">
         <v>985.2</v>
       </c>
-      <c r="L42" s="62"/>
-      <c r="M42" s="64"/>
-      <c r="N42" s="62"/>
-      <c r="O42" s="40">
+      <c r="L42" s="40">
+        <v>985.2</v>
+      </c>
+      <c r="M42" s="58"/>
+      <c r="N42" s="61"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="40">
         <v>0.89</v>
       </c>
-      <c r="P42" s="40">
+      <c r="Q42" s="40">
         <f t="shared" si="0"/>
-        <v>876.82799999999997</v>
-      </c>
-      <c r="Q42" s="42" t="s">
+        <v>876.82800000000009</v>
+      </c>
+      <c r="R42" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R42" s="40"/>
-      <c r="S42" s="40" t="s">
+      <c r="S42" s="40"/>
+      <c r="T42" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="T42" s="52">
+      <c r="U42" s="52">
         <f>1.05*0.85</f>
         <v>0.89249999999999996</v>
       </c>
-      <c r="U42" s="55">
+      <c r="V42" s="55">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V42" s="56">
+      <c r="W42" s="56">
         <f t="shared" si="4"/>
-        <v>-2.4999999999999502E-3</v>
-      </c>
-      <c r="W42" s="52">
+        <v>-2.4999999999999467E-3</v>
+      </c>
+      <c r="X42" s="52">
         <f>1.05*0.85</f>
         <v>0.89249999999999996</v>
       </c>
-      <c r="X42" s="54"/>
       <c r="Y42" s="54"/>
       <c r="Z42" s="54"/>
-      <c r="AB42" s="54"/>
-    </row>
-    <row r="43" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA42" s="54"/>
+      <c r="AC42" s="54"/>
+    </row>
+    <row r="43" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A43" s="20" t="s">
         <v>95</v>
       </c>
@@ -4063,41 +4209,44 @@
       <c r="K43" s="40">
         <v>2828.1</v>
       </c>
-      <c r="L43" s="61">
+      <c r="L43" s="40">
+        <v>2828.1</v>
+      </c>
+      <c r="M43" s="59">
         <v>1</v>
       </c>
-      <c r="M43" s="63">
+      <c r="N43" s="60">
         <v>317.5</v>
       </c>
-      <c r="N43" s="66">
+      <c r="O43" s="57">
         <v>362.5</v>
       </c>
-      <c r="O43" s="40">
+      <c r="P43" s="40">
         <v>1.05</v>
       </c>
-      <c r="P43" s="40">
+      <c r="Q43" s="40">
         <f t="shared" si="0"/>
         <v>2969.5050000000001</v>
       </c>
-      <c r="Q43" s="42" t="s">
+      <c r="R43" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R43" s="40" t="s">
+      <c r="S43" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="S43" s="40" t="s">
+      <c r="T43" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="T43" s="52"/>
-      <c r="U43" s="55"/>
-      <c r="V43" s="56"/>
-      <c r="W43" s="52"/>
-      <c r="X43" s="54"/>
+      <c r="U43" s="52"/>
+      <c r="V43" s="55"/>
+      <c r="W43" s="56"/>
+      <c r="X43" s="52"/>
       <c r="Y43" s="54"/>
       <c r="Z43" s="54"/>
-      <c r="AB43" s="54"/>
-    </row>
-    <row r="44" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA43" s="54"/>
+      <c r="AC43" s="54"/>
+    </row>
+    <row r="44" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A44" s="20" t="s">
         <v>95</v>
       </c>
@@ -4129,45 +4278,48 @@
       <c r="K44" s="40">
         <v>782.6</v>
       </c>
-      <c r="L44" s="62"/>
-      <c r="M44" s="64"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="40">
+      <c r="L44" s="40">
+        <v>782.6</v>
+      </c>
+      <c r="M44" s="58"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="40">
         <v>0.95</v>
       </c>
-      <c r="P44" s="40">
+      <c r="Q44" s="40">
         <f t="shared" si="0"/>
         <v>743.47</v>
       </c>
-      <c r="Q44" s="42" t="s">
+      <c r="R44" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40" t="s">
+      <c r="S44" s="40"/>
+      <c r="T44" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="T44" s="52">
-        <f t="shared" ref="T44:T48" si="5">1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="U44" s="55">
+      <c r="U44" s="52">
+        <f t="shared" ref="U44:U48" si="5">1.05*0.9</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V44" s="55">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V44" s="56">
+      <c r="W44" s="56">
         <f t="shared" si="4"/>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W44" s="52">
-        <f t="shared" ref="W44:W48" si="6">1.05*0.9</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="X44" s="54"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X44" s="52">
+        <f t="shared" ref="X44:X48" si="6">1.05*0.9</f>
+        <v>0.94500000000000006</v>
+      </c>
       <c r="Y44" s="54"/>
       <c r="Z44" s="54"/>
-      <c r="AB44" s="54"/>
-    </row>
-    <row r="45" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA44" s="54"/>
+      <c r="AC44" s="54"/>
+    </row>
+    <row r="45" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A45" s="20" t="s">
         <v>83</v>
       </c>
@@ -4199,41 +4351,44 @@
       <c r="K45" s="40">
         <v>9986.6</v>
       </c>
-      <c r="L45" s="61">
+      <c r="L45" s="40">
+        <v>9986.6</v>
+      </c>
+      <c r="M45" s="59">
         <v>1</v>
       </c>
-      <c r="M45" s="63">
+      <c r="N45" s="60">
         <v>965.5</v>
       </c>
-      <c r="N45" s="66">
+      <c r="O45" s="57">
         <v>1010.5</v>
       </c>
-      <c r="O45" s="40">
+      <c r="P45" s="40">
         <v>1.05</v>
       </c>
-      <c r="P45" s="40">
+      <c r="Q45" s="40">
         <f t="shared" si="0"/>
         <v>10485.93</v>
       </c>
-      <c r="Q45" s="42" t="s">
+      <c r="R45" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R45" s="40" t="s">
+      <c r="S45" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="S45" s="40" t="s">
+      <c r="T45" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="T45" s="52"/>
-      <c r="U45" s="55"/>
-      <c r="V45" s="56"/>
-      <c r="W45" s="52"/>
-      <c r="X45" s="54"/>
+      <c r="U45" s="52"/>
+      <c r="V45" s="55"/>
+      <c r="W45" s="56"/>
+      <c r="X45" s="52"/>
       <c r="Y45" s="54"/>
       <c r="Z45" s="54"/>
-      <c r="AB45" s="54"/>
-    </row>
-    <row r="46" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA45" s="54"/>
+      <c r="AC45" s="54"/>
+    </row>
+    <row r="46" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A46" s="20" t="s">
         <v>83</v>
       </c>
@@ -4265,45 +4420,48 @@
       <c r="K46" s="40">
         <v>794.1</v>
       </c>
-      <c r="L46" s="62"/>
-      <c r="M46" s="64"/>
-      <c r="N46" s="62"/>
-      <c r="O46" s="40">
+      <c r="L46" s="40">
+        <v>794.1</v>
+      </c>
+      <c r="M46" s="58"/>
+      <c r="N46" s="61"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="40">
         <v>0.95</v>
       </c>
-      <c r="P46" s="40">
+      <c r="Q46" s="40">
         <f t="shared" si="0"/>
         <v>754.39499999999998</v>
       </c>
-      <c r="Q46" s="42" t="s">
+      <c r="R46" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R46" s="40"/>
-      <c r="S46" s="40" t="s">
+      <c r="S46" s="40"/>
+      <c r="T46" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="T46" s="52">
+      <c r="U46" s="52">
         <f t="shared" si="5"/>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="U46" s="55">
-        <f>T46-W46</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V46" s="55">
+        <f>U46-X46</f>
         <v>0</v>
       </c>
-      <c r="V46" s="56">
-        <f>O46-T46</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W46" s="52">
+      <c r="W46" s="56">
+        <f>P46-U46</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X46" s="52">
         <f t="shared" si="6"/>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="X46" s="54"/>
+        <v>0.94500000000000006</v>
+      </c>
       <c r="Y46" s="54"/>
       <c r="Z46" s="54"/>
-      <c r="AB46" s="54"/>
-    </row>
-    <row r="47" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA46" s="54"/>
+      <c r="AC46" s="54"/>
+    </row>
+    <row r="47" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A47" s="20" t="s">
         <v>83</v>
       </c>
@@ -4335,41 +4493,44 @@
       <c r="K47" s="40">
         <v>9379.6</v>
       </c>
-      <c r="L47" s="61">
+      <c r="L47" s="40">
+        <v>9379.6</v>
+      </c>
+      <c r="M47" s="59">
         <v>1</v>
       </c>
-      <c r="M47" s="63">
+      <c r="N47" s="60">
         <v>971</v>
       </c>
-      <c r="N47" s="66">
+      <c r="O47" s="57">
         <v>1016</v>
       </c>
-      <c r="O47" s="40">
+      <c r="P47" s="40">
         <v>1.05</v>
       </c>
-      <c r="P47" s="40">
+      <c r="Q47" s="40">
         <f t="shared" si="0"/>
         <v>9848.58</v>
       </c>
-      <c r="Q47" s="42" t="s">
+      <c r="R47" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R47" s="40" t="s">
+      <c r="S47" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="S47" s="40" t="s">
+      <c r="T47" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="T47" s="52"/>
-      <c r="U47" s="55"/>
-      <c r="V47" s="56"/>
-      <c r="W47" s="52"/>
-      <c r="X47" s="54"/>
+      <c r="U47" s="52"/>
+      <c r="V47" s="55"/>
+      <c r="W47" s="56"/>
+      <c r="X47" s="52"/>
       <c r="Y47" s="54"/>
       <c r="Z47" s="54"/>
-      <c r="AB47" s="54"/>
-    </row>
-    <row r="48" spans="1:28" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="AA47" s="54"/>
+      <c r="AC47" s="54"/>
+    </row>
+    <row r="48" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
       <c r="A48" s="20" t="s">
         <v>83</v>
       </c>
@@ -4401,47 +4562,50 @@
       <c r="K48" s="40">
         <v>1572.9</v>
       </c>
-      <c r="L48" s="62"/>
-      <c r="M48" s="64"/>
-      <c r="N48" s="62"/>
-      <c r="O48" s="40">
+      <c r="L48" s="40">
+        <v>1572.9</v>
+      </c>
+      <c r="M48" s="58"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="40">
         <v>0.95</v>
       </c>
-      <c r="P48" s="40">
+      <c r="Q48" s="40">
         <f t="shared" si="0"/>
         <v>1494.2550000000001</v>
       </c>
-      <c r="Q48" s="42" t="s">
+      <c r="R48" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="R48" s="40"/>
-      <c r="S48" s="40" t="s">
+      <c r="S48" s="40"/>
+      <c r="T48" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="T48" s="52">
+      <c r="U48" s="52">
         <f t="shared" si="5"/>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="U48" s="55">
-        <f>T48-W48</f>
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="V48" s="55">
+        <f>U48-X48</f>
         <v>0</v>
       </c>
-      <c r="V48" s="56">
-        <f>O48-T48</f>
-        <v>4.9999999999998899E-3</v>
-      </c>
-      <c r="W48" s="52">
+      <c r="W48" s="56">
+        <f>P48-U48</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="X48" s="52">
         <f t="shared" si="6"/>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="X48" s="54"/>
+        <v>0.94500000000000006</v>
+      </c>
       <c r="Y48" s="54"/>
       <c r="Z48" s="54"/>
-      <c r="AB48" s="54"/>
-    </row>
-    <row r="49" spans="10:16">
+      <c r="AA48" s="54"/>
+      <c r="AC48" s="54"/>
+    </row>
+    <row r="49" spans="1:29">
       <c r="J49">
-        <f t="shared" ref="J49:L49" si="7">SUM(J10:J48)</f>
+        <f t="shared" ref="J49:M49" si="7">SUM(J10:J48)</f>
         <v>4778</v>
       </c>
       <c r="K49">
@@ -4449,49 +4613,1079 @@
         <v>252596.8</v>
       </c>
       <c r="L49">
+        <f t="shared" ref="L49" si="8">SUM(L10:L48)</f>
+        <v>252596.8</v>
+      </c>
+      <c r="M49">
         <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="P49">
-        <f>SUM(P10:P48)</f>
-        <v>294595.24400000001</v>
-      </c>
+      <c r="Q49">
+        <f>SUM(Q10:Q48)</f>
+        <v>294595.24400000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" s="3" customFormat="1" ht="45" customHeight="1">
+      <c r="A50" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J50" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K50" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M50" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O50" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="P50" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q50" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="R50" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="U50" s="51"/>
+    </row>
+    <row r="51" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A51" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G51" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H51" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" s="40">
+        <v>190</v>
+      </c>
+      <c r="K51" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="L51" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="M51" s="40">
+        <v>1</v>
+      </c>
+      <c r="N51" s="41">
+        <f>O51-45</f>
+        <v>768.5</v>
+      </c>
+      <c r="O51" s="42">
+        <v>813.5</v>
+      </c>
+      <c r="P51" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q51" s="40">
+        <f t="shared" ref="Q51:Q54" si="9">P51*K51</f>
+        <v>12761.625</v>
+      </c>
+      <c r="R51" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S51" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="T51" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="U51" s="52"/>
+      <c r="V51" s="53"/>
+      <c r="W51" s="52"/>
+      <c r="X51" s="52"/>
+      <c r="Y51" s="54"/>
+      <c r="Z51" s="54"/>
+      <c r="AA51" s="54"/>
+      <c r="AC51" s="54"/>
+    </row>
+    <row r="52" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A52" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H52" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J52" s="40">
+        <v>135</v>
+      </c>
+      <c r="K52" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="L52" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="M52" s="40">
+        <v>1</v>
+      </c>
+      <c r="N52" s="41">
+        <f>O52-45</f>
+        <v>568.5</v>
+      </c>
+      <c r="O52" s="42">
+        <v>613.5</v>
+      </c>
+      <c r="P52" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q52" s="40">
+        <f t="shared" si="9"/>
+        <v>9247.75</v>
+      </c>
+      <c r="R52" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S52" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="T52" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="U52" s="52"/>
+      <c r="V52" s="53"/>
+      <c r="W52" s="52"/>
+      <c r="X52" s="52"/>
+      <c r="Y52" s="54"/>
+      <c r="Z52" s="54"/>
+      <c r="AA52" s="54"/>
+      <c r="AC52" s="54"/>
+    </row>
+    <row r="53" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A53" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C53" s="21">
+        <v>20</v>
+      </c>
+      <c r="D53" s="22"/>
+      <c r="E53" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F53" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H53" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J53" s="40">
+        <v>200</v>
+      </c>
+      <c r="K53" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="L53" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="M53" s="40">
+        <v>1</v>
+      </c>
+      <c r="N53" s="41">
+        <v>835.5</v>
+      </c>
+      <c r="O53" s="42">
+        <v>880.5</v>
+      </c>
+      <c r="P53" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q53" s="40">
+        <f t="shared" si="9"/>
+        <v>13405.875</v>
+      </c>
+      <c r="R53" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S53" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="T53" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="U53" s="52"/>
+      <c r="V53" s="53"/>
+      <c r="W53" s="52"/>
+      <c r="X53" s="52"/>
+      <c r="Y53" s="54"/>
+      <c r="Z53" s="54"/>
+      <c r="AA53" s="54"/>
+      <c r="AC53" s="54"/>
+    </row>
+    <row r="54" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A54" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C54" s="21">
+        <v>20</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G54" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H54" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J54" s="40">
+        <v>200</v>
+      </c>
+      <c r="K54" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="L54" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="M54" s="40">
+        <v>1</v>
+      </c>
+      <c r="N54" s="41">
+        <v>816</v>
+      </c>
+      <c r="O54" s="42">
+        <v>861</v>
+      </c>
+      <c r="P54" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q54" s="40">
+        <f t="shared" si="9"/>
+        <v>13359</v>
+      </c>
+      <c r="R54" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S54" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="T54" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="U54" s="52"/>
+      <c r="V54" s="53"/>
+      <c r="W54" s="52"/>
+      <c r="X54" s="52"/>
+      <c r="Y54" s="54"/>
+      <c r="Z54" s="54"/>
+      <c r="AA54" s="54"/>
+      <c r="AC54" s="54"/>
+    </row>
+    <row r="58" spans="1:29" s="3" customFormat="1" ht="45" customHeight="1">
+      <c r="A58" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K58" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L58" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M58" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O58" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="P58" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q58" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="R58" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="S58" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="U58" s="51"/>
+    </row>
+    <row r="59" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A59" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E59" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F59" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" s="40">
+        <v>190</v>
+      </c>
+      <c r="K59" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="L59" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="M59" s="40">
+        <v>1</v>
+      </c>
+      <c r="N59" s="41">
+        <f>O59-45</f>
+        <v>768.5</v>
+      </c>
+      <c r="O59" s="42">
+        <v>813.5</v>
+      </c>
+      <c r="P59" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q59" s="40">
+        <f t="shared" ref="Q59:Q62" si="10">P59*K59</f>
+        <v>12761.625</v>
+      </c>
+      <c r="R59" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S59" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="T59" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="U59" s="52"/>
+      <c r="V59" s="53"/>
+      <c r="W59" s="52"/>
+      <c r="X59" s="52"/>
+      <c r="Y59" s="54"/>
+      <c r="Z59" s="54"/>
+      <c r="AA59" s="54"/>
+      <c r="AC59" s="54"/>
+    </row>
+    <row r="60" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A60" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I60" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="40">
+        <v>135</v>
+      </c>
+      <c r="K60" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="L60" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="M60" s="40">
+        <v>1</v>
+      </c>
+      <c r="N60" s="41">
+        <f>O60-45</f>
+        <v>568.5</v>
+      </c>
+      <c r="O60" s="42">
+        <v>613.5</v>
+      </c>
+      <c r="P60" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q60" s="40">
+        <f t="shared" si="10"/>
+        <v>9247.75</v>
+      </c>
+      <c r="R60" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S60" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="T60" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="U60" s="52"/>
+      <c r="V60" s="53"/>
+      <c r="W60" s="52"/>
+      <c r="X60" s="52"/>
+      <c r="Y60" s="54"/>
+      <c r="Z60" s="54"/>
+      <c r="AA60" s="54"/>
+      <c r="AC60" s="54"/>
+    </row>
+    <row r="61" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A61" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C61" s="21">
+        <v>20</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H61" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I61" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J61" s="40">
+        <v>200</v>
+      </c>
+      <c r="K61" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="L61" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="M61" s="40">
+        <v>1</v>
+      </c>
+      <c r="N61" s="41">
+        <v>835.5</v>
+      </c>
+      <c r="O61" s="42">
+        <v>880.5</v>
+      </c>
+      <c r="P61" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q61" s="40">
+        <f t="shared" si="10"/>
+        <v>13405.875</v>
+      </c>
+      <c r="R61" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S61" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="T61" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="U61" s="52"/>
+      <c r="V61" s="53"/>
+      <c r="W61" s="52"/>
+      <c r="X61" s="52"/>
+      <c r="Y61" s="54"/>
+      <c r="Z61" s="54"/>
+      <c r="AA61" s="54"/>
+      <c r="AC61" s="54"/>
+    </row>
+    <row r="62" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A62" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B62" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C62" s="21">
+        <v>20</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I62" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J62" s="40">
+        <v>200</v>
+      </c>
+      <c r="K62" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="L62" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="M62" s="40">
+        <v>1</v>
+      </c>
+      <c r="N62" s="41">
+        <v>816</v>
+      </c>
+      <c r="O62" s="42">
+        <v>861</v>
+      </c>
+      <c r="P62" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q62" s="40">
+        <f t="shared" si="10"/>
+        <v>13359</v>
+      </c>
+      <c r="R62" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S62" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="T62" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="U62" s="52"/>
+      <c r="V62" s="53"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="54"/>
+      <c r="Z62" s="54"/>
+      <c r="AA62" s="54"/>
+      <c r="AC62" s="54"/>
+    </row>
+    <row r="65" spans="1:29" s="3" customFormat="1" ht="45" customHeight="1">
+      <c r="A65" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I65" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J65" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K65" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L65" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M65" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="N65" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O65" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="P65" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q65" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="R65" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="S65" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="U65" s="51"/>
+    </row>
+    <row r="66" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A66" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I66" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J66" s="40">
+        <v>190</v>
+      </c>
+      <c r="K66" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="L66" s="40">
+        <v>10209.299999999999</v>
+      </c>
+      <c r="M66" s="40">
+        <v>1</v>
+      </c>
+      <c r="N66" s="41">
+        <f>O66-45</f>
+        <v>768.5</v>
+      </c>
+      <c r="O66" s="42">
+        <v>813.5</v>
+      </c>
+      <c r="P66" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q66" s="40">
+        <f t="shared" ref="Q66:Q69" si="11">P66*K66</f>
+        <v>12761.625</v>
+      </c>
+      <c r="R66" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S66" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="T66" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="U66" s="52"/>
+      <c r="V66" s="53"/>
+      <c r="W66" s="52"/>
+      <c r="X66" s="52"/>
+      <c r="Y66" s="54"/>
+      <c r="Z66" s="54"/>
+      <c r="AA66" s="54"/>
+      <c r="AC66" s="54"/>
+    </row>
+    <row r="67" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A67" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="23">
+        <v>45799</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H67" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I67" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J67" s="40">
+        <v>135</v>
+      </c>
+      <c r="K67" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="L67" s="40">
+        <v>7398.2</v>
+      </c>
+      <c r="M67" s="40">
+        <v>1</v>
+      </c>
+      <c r="N67" s="41">
+        <f>O67-45</f>
+        <v>568.5</v>
+      </c>
+      <c r="O67" s="42">
+        <v>613.5</v>
+      </c>
+      <c r="P67" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q67" s="40">
+        <f t="shared" si="11"/>
+        <v>9247.75</v>
+      </c>
+      <c r="R67" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S67" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="T67" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="U67" s="52"/>
+      <c r="V67" s="53"/>
+      <c r="W67" s="52"/>
+      <c r="X67" s="52"/>
+      <c r="Y67" s="54"/>
+      <c r="Z67" s="54"/>
+      <c r="AA67" s="54"/>
+      <c r="AC67" s="54"/>
+    </row>
+    <row r="68" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A68" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C68" s="21">
+        <v>20</v>
+      </c>
+      <c r="D68" s="22"/>
+      <c r="E68" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G68" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I68" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J68" s="40">
+        <v>200</v>
+      </c>
+      <c r="K68" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="L68" s="40">
+        <v>10724.7</v>
+      </c>
+      <c r="M68" s="40">
+        <v>1</v>
+      </c>
+      <c r="N68" s="41">
+        <v>835.5</v>
+      </c>
+      <c r="O68" s="42">
+        <v>880.5</v>
+      </c>
+      <c r="P68" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q68" s="40">
+        <f t="shared" si="11"/>
+        <v>13405.875</v>
+      </c>
+      <c r="R68" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S68" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="T68" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="U68" s="52"/>
+      <c r="V68" s="53"/>
+      <c r="W68" s="52"/>
+      <c r="X68" s="52"/>
+      <c r="Y68" s="54"/>
+      <c r="Z68" s="54"/>
+      <c r="AA68" s="54"/>
+      <c r="AC68" s="54"/>
+    </row>
+    <row r="69" spans="1:29" s="4" customFormat="1" ht="45" customHeight="1">
+      <c r="A69" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" s="21">
+        <v>9000714968</v>
+      </c>
+      <c r="C69" s="21">
+        <v>20</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="23">
+        <v>45827</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G69" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I69" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" s="40">
+        <v>200</v>
+      </c>
+      <c r="K69" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="L69" s="40">
+        <v>10687.2</v>
+      </c>
+      <c r="M69" s="40">
+        <v>1</v>
+      </c>
+      <c r="N69" s="41">
+        <v>816</v>
+      </c>
+      <c r="O69" s="42">
+        <v>861</v>
+      </c>
+      <c r="P69" s="40">
+        <v>1.25</v>
+      </c>
+      <c r="Q69" s="40">
+        <f t="shared" si="11"/>
+        <v>13359</v>
+      </c>
+      <c r="R69" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="S69" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="T69" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="U69" s="52"/>
+      <c r="V69" s="53"/>
+      <c r="W69" s="52"/>
+      <c r="X69" s="52"/>
+      <c r="Y69" s="54"/>
+      <c r="Z69" s="54"/>
+      <c r="AA69" s="54"/>
+      <c r="AC69" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="G1:J4"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="M47:M48"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="N27:N29"/>
+    <mergeCell ref="N33:N35"/>
     <mergeCell ref="N39:N40"/>
     <mergeCell ref="N41:N42"/>
     <mergeCell ref="N43:N44"/>
     <mergeCell ref="N45:N46"/>
     <mergeCell ref="N47:N48"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="N27:N29"/>
-    <mergeCell ref="N33:N35"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="M25:M26"/>
     <mergeCell ref="M27:M29"/>
     <mergeCell ref="M33:M35"/>
     <mergeCell ref="M39:M40"/>
     <mergeCell ref="M41:M42"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="M47:M48"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="G1:J4"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="O27:O29"/>
+    <mergeCell ref="O33:O35"/>
+    <mergeCell ref="O39:O40"/>
+    <mergeCell ref="O41:O42"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="O47:O48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>